<commit_message>
Added look into different age comparisons of the data and varying vaccine definitions
</commit_message>
<xml_diff>
--- a/Vaccine Case Control Analysis/TCV_VE_analysis_model_results.xlsx
+++ b/Vaccine Case Control Analysis/TCV_VE_analysis_model_results.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ChrisLeBoa/GitHub/typhoid_research/india_typhoid/Vaccine Case Control Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29CE748D-02CD-0A44-827E-C773F868C0F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB5A0E65-7082-C44E-999F-7C175DE9AB90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23600" yWindow="0" windowWidth="10000" windowHeight="21000" xr2:uid="{3EDAAADB-6F96-FC4A-BED9-FC7DD87A3A84}"/>
+    <workbookView xWindow="14080" yWindow="960" windowWidth="17800" windowHeight="18980" xr2:uid="{3EDAAADB-6F96-FC4A-BED9-FC7DD87A3A84}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>OR</t>
   </si>
@@ -84,9 +84,6 @@
   </si>
   <si>
     <t>Any typhoid vaccine reported</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Any TCV reported (not specified how defined in codebook) </t>
   </si>
 </sst>
 </file>
@@ -445,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ADD5A4E-EEFF-F441-82E8-BF39AFB4092C}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -546,15 +543,15 @@
         <v>0.42520000000000002</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H8" si="0">1-E3</f>
+        <f t="shared" ref="H3:H7" si="0">1-E3</f>
         <v>0.876</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I8" si="1">1-F3</f>
+        <f t="shared" ref="I3:I7" si="1">1-F3</f>
         <v>0.96340000000000003</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J8" si="2">1-G3</f>
+        <f t="shared" ref="J3:J7" si="2">1-G3</f>
         <v>0.57479999999999998</v>
       </c>
     </row>
@@ -595,134 +592,99 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5">
+        <v>40</v>
+      </c>
+      <c r="C5">
         <v>37</v>
       </c>
-      <c r="C5">
-        <v>34</v>
-      </c>
       <c r="D5">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="E5">
-        <v>0.372</v>
+        <v>0.33850000000000002</v>
       </c>
       <c r="F5">
-        <v>0.155</v>
+        <v>0.153</v>
       </c>
       <c r="G5">
-        <v>0.89300000000000002</v>
+        <v>0.75</v>
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
-        <v>0.628</v>
+        <v>0.66149999999999998</v>
       </c>
       <c r="I5">
         <f t="shared" si="1"/>
-        <v>0.84499999999999997</v>
+        <v>0.84699999999999998</v>
       </c>
       <c r="J5">
         <f t="shared" si="2"/>
-        <v>0.10699999999999998</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="C6">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="D6">
-        <v>148</v>
+        <v>33</v>
       </c>
       <c r="E6">
-        <v>0.33850000000000002</v>
+        <v>0.27650000000000002</v>
       </c>
       <c r="F6">
-        <v>0.153</v>
+        <v>3.1329999999999997E-2</v>
       </c>
       <c r="G6">
-        <v>0.75</v>
+        <v>2.44</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>0.66149999999999998</v>
+        <v>0.72350000000000003</v>
       </c>
       <c r="I6">
         <f t="shared" si="1"/>
-        <v>0.84699999999999998</v>
+        <v>0.96867000000000003</v>
       </c>
       <c r="J6">
         <f t="shared" si="2"/>
-        <v>0.25</v>
+        <v>-1.44</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D7">
-        <v>33</v>
+        <v>107</v>
       </c>
       <c r="E7">
-        <v>0.27650000000000002</v>
+        <v>0.12959999999999999</v>
       </c>
       <c r="F7">
-        <v>3.1329999999999997E-2</v>
+        <v>2.9399999999999999E-2</v>
       </c>
       <c r="G7">
-        <v>2.44</v>
+        <v>0.57120000000000004</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>0.72350000000000003</v>
+        <v>0.87040000000000006</v>
       </c>
       <c r="I7">
         <f t="shared" si="1"/>
-        <v>0.96867000000000003</v>
+        <v>0.97060000000000002</v>
       </c>
       <c r="J7">
-        <f t="shared" si="2"/>
-        <v>-1.44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8">
-        <v>27</v>
-      </c>
-      <c r="D8">
-        <v>107</v>
-      </c>
-      <c r="E8">
-        <v>0.12959999999999999</v>
-      </c>
-      <c r="F8">
-        <v>2.9399999999999999E-2</v>
-      </c>
-      <c r="G8">
-        <v>0.57120000000000004</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="0"/>
-        <v>0.87040000000000006</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="1"/>
-        <v>0.97060000000000002</v>
-      </c>
-      <c r="J8">
         <f t="shared" si="2"/>
         <v>0.42879999999999996</v>
       </c>

</xml_diff>